<commit_message>
Added vSPD results for 13pt7MWh
</commit_message>
<xml_diff>
--- a/vSPD_data/EXCEL_FILES/vSPD_UTS_daily_system_load_cost_results.xlsx
+++ b/vSPD_data/EXCEL_FILES/vSPD_UTS_daily_system_load_cost_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>vSPD LSI offers@$10/MWh</t>
+  </si>
+  <si>
+    <t>vSPD LSI offers@$13.7/MWh</t>
   </si>
   <si>
     <t>vSPD LSI offers@$20/MWh</t>
@@ -389,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -397,7 +400,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,8 +422,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="n">
         <v>43778</v>
       </c>
@@ -429,11 +435,12 @@
       <c r="D2" t="s"/>
       <c r="E2" t="s"/>
       <c r="F2" t="s"/>
-      <c r="G2" t="n">
+      <c r="G2" t="s"/>
+      <c r="H2" t="n">
         <v>11.39289576</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="n">
         <v>43779</v>
       </c>
@@ -444,19 +451,22 @@
         <v>11.12763769</v>
       </c>
       <c r="D3" t="n">
+        <v>11.12763769</v>
+      </c>
+      <c r="E3" t="n">
         <v>7.69390488</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>8.138274299999999</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>11.12763769</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>11.59799322</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="n">
         <v>43780</v>
       </c>
@@ -467,19 +477,22 @@
         <v>9.8506315</v>
       </c>
       <c r="D4" t="n">
+        <v>9.860017060000001</v>
+      </c>
+      <c r="E4" t="n">
         <v>8.038879</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>8.463236009999999</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>9.82801969</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>9.82435772</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="n">
         <v>43781</v>
       </c>
@@ -490,19 +503,22 @@
         <v>11.6806809</v>
       </c>
       <c r="D5" t="n">
+        <v>11.6806809</v>
+      </c>
+      <c r="E5" t="n">
         <v>9.427818960000002</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>9.843790779999999</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>11.6806809</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>11.69183748</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="n">
         <v>43782</v>
       </c>
@@ -513,19 +529,22 @@
         <v>7.25098188</v>
       </c>
       <c r="D6" t="n">
+        <v>7.3250106</v>
+      </c>
+      <c r="E6" t="n">
         <v>5.97113642</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>6.3411703</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>7.108060490000001</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>7.57593392</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="n">
         <v>43783</v>
       </c>
@@ -536,19 +555,22 @@
         <v>6.905957320000001</v>
       </c>
       <c r="D7" t="n">
+        <v>6.97784897</v>
+      </c>
+      <c r="E7" t="n">
         <v>5.60272109</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>6.09082304</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>6.70452871</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>7.21131766</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="n">
         <v>43784</v>
       </c>
@@ -559,19 +581,22 @@
         <v>6.223123599999999</v>
       </c>
       <c r="D8" t="n">
+        <v>6.2909372</v>
+      </c>
+      <c r="E8" t="n">
         <v>4.01576939</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>4.79020736</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>6.09978788</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>7.18856881</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="n">
         <v>43785</v>
       </c>
@@ -582,19 +607,22 @@
         <v>3.02713028</v>
       </c>
       <c r="D9" t="n">
+        <v>4.8386023</v>
+      </c>
+      <c r="E9" t="n">
         <v>3.68792326</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>4.34784695</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>4.46091015</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>6.647664509999999</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="n">
         <v>43786</v>
       </c>
@@ -605,19 +633,22 @@
         <v>4.46874795</v>
       </c>
       <c r="D10" t="n">
+        <v>6.16493004</v>
+      </c>
+      <c r="E10" t="n">
         <v>5.01959757</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>5.51742627</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>5.82779063</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>7.37751206</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="n">
         <v>43787</v>
       </c>
@@ -628,19 +659,22 @@
         <v>8.562618720000001</v>
       </c>
       <c r="D11" t="n">
+        <v>7.9942987</v>
+      </c>
+      <c r="E11" t="n">
         <v>8.95078217</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>9.341532689999999</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>7.72353366</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>11.46491868</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="n">
         <v>43788</v>
       </c>
@@ -650,20 +684,21 @@
       <c r="C12" t="n">
         <v>6.33041139</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" t="s"/>
+      <c r="E12" t="n">
         <v>6.65290392</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>6.97169189</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>5.53438269</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>8.06572723</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="2" t="n">
         <v>43789</v>
       </c>
@@ -674,19 +709,22 @@
         <v>8.58000024</v>
       </c>
       <c r="D13" t="n">
+        <v>8.661373279999999</v>
+      </c>
+      <c r="E13" t="n">
         <v>7.35702113</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>7.75641005</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>8.420270090000001</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>9.676797890000001</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" s="2" t="n">
         <v>43790</v>
       </c>
@@ -697,19 +735,22 @@
         <v>13.40225945</v>
       </c>
       <c r="D14" t="n">
+        <v>13.40225945</v>
+      </c>
+      <c r="E14" t="n">
         <v>10.32755392</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>10.66805026</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>13.40225945</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>13.90543526</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" s="2" t="n">
         <v>43791</v>
       </c>
@@ -720,19 +761,22 @@
         <v>6.525188320000001</v>
       </c>
       <c r="D15" t="n">
+        <v>6.59054157</v>
+      </c>
+      <c r="E15" t="n">
         <v>5.19635942</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>5.78914961</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>6.38144231</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>7.30337867</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" s="2" t="n">
         <v>43792</v>
       </c>
@@ -743,19 +787,22 @@
         <v>5.71666164</v>
       </c>
       <c r="D16" t="n">
+        <v>5.81657908</v>
+      </c>
+      <c r="E16" t="n">
         <v>4.72974925</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>5.16639524</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>5.46252233</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>7.0173548</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" s="2" t="n">
         <v>43793</v>
       </c>
@@ -766,19 +813,22 @@
         <v>5.63514456</v>
       </c>
       <c r="D17" t="n">
+        <v>5.71759337</v>
+      </c>
+      <c r="E17" t="n">
         <v>3.68132314</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>4.48300155</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>5.44057351</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>7.056666219999999</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" s="2" t="n">
         <v>43794</v>
       </c>
@@ -789,19 +839,22 @@
         <v>10.59468009</v>
       </c>
       <c r="D18" t="n">
+        <v>10.59285637</v>
+      </c>
+      <c r="E18" t="n">
         <v>7.797578929999999</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>8.28172092</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>10.59960416</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>12.00410536</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" s="2" t="n">
         <v>43795</v>
       </c>
@@ -812,19 +865,22 @@
         <v>10.32763701</v>
       </c>
       <c r="D19" t="n">
+        <v>10.32387422</v>
+      </c>
+      <c r="E19" t="n">
         <v>8.03639701</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>8.506707109999999</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>10.33813522</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>11.88520596</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" s="2" t="n">
         <v>43796</v>
       </c>
@@ -835,19 +891,22 @@
         <v>9.900359699999999</v>
       </c>
       <c r="D20" t="n">
+        <v>9.90063074</v>
+      </c>
+      <c r="E20" t="n">
         <v>8.1490492</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>8.50272077</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>9.902875949999999</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>10.54031936</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21" s="2" t="n">
         <v>43797</v>
       </c>
@@ -858,19 +917,22 @@
         <v>12.50287627</v>
       </c>
       <c r="D21" t="n">
+        <v>12.53261627</v>
+      </c>
+      <c r="E21" t="n">
         <v>11.32630816</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>11.70023058</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>12.42567294</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>15.32649178</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22" s="2" t="n">
         <v>43798</v>
       </c>
@@ -881,19 +943,22 @@
         <v>11.25419693</v>
       </c>
       <c r="D22" t="n">
+        <v>11.2541515</v>
+      </c>
+      <c r="E22" t="n">
         <v>9.821660830000001</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>10.1746227</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>11.25419693</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>13.45711161</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="A23" s="2" t="n">
         <v>43799</v>
       </c>
@@ -904,19 +969,22 @@
         <v>12.31017436</v>
       </c>
       <c r="D23" t="n">
+        <v>12.31017436</v>
+      </c>
+      <c r="E23" t="n">
         <v>10.29985852</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>10.68466594</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>12.31017436</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>12.43671474</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8">
       <c r="A24" s="2" t="n">
         <v>43800</v>
       </c>
@@ -927,19 +995,22 @@
         <v>7.29087128</v>
       </c>
       <c r="D24" t="n">
+        <v>7.3044338</v>
+      </c>
+      <c r="E24" t="n">
         <v>5.75441577</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>6.2128798</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>7.29087128</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>7.890002440000001</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="A25" s="2" t="n">
         <v>43801</v>
       </c>
@@ -950,19 +1021,22 @@
         <v>16.83043186</v>
       </c>
       <c r="D25" t="n">
+        <v>16.89880727</v>
+      </c>
+      <c r="E25" t="n">
         <v>14.66291678</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>15.05856505</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>16.65759468</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>17.26557853</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8">
       <c r="A26" s="2" t="n">
         <v>43802</v>
       </c>
@@ -973,19 +1047,22 @@
         <v>2.30711758</v>
       </c>
       <c r="D26" t="n">
+        <v>2.64570165</v>
+      </c>
+      <c r="E26" t="n">
         <v>3.20831549</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>4.29498349</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>1.93572928</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>8.531145689999999</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8">
       <c r="A27" s="2" t="n">
         <v>43803</v>
       </c>
@@ -996,19 +1073,22 @@
         <v>4.201692400000001</v>
       </c>
       <c r="D27" t="n">
+        <v>4.406702070000001</v>
+      </c>
+      <c r="E27" t="n">
         <v>4.799231</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>5.47240638</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>4.01223046</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>9.641018240000001</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="A28" s="2" t="n">
         <v>43804</v>
       </c>
@@ -1019,19 +1099,22 @@
         <v>5.06001278</v>
       </c>
       <c r="D28" t="n">
+        <v>5.241911849999999</v>
+      </c>
+      <c r="E28" t="n">
         <v>5.60131805</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>6.17162613</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>4.89563448</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>11.39652988</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:8">
       <c r="A29" s="2" t="n">
         <v>43805</v>
       </c>
@@ -1042,19 +1125,22 @@
         <v>5.59766862</v>
       </c>
       <c r="D29" t="n">
+        <v>5.84174483</v>
+      </c>
+      <c r="E29" t="n">
         <v>6.269095549999999</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>6.99406259</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>5.360284900000001</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>12.28941343</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30" s="2" t="n">
         <v>43806</v>
       </c>
@@ -1065,19 +1151,22 @@
         <v>3.0440999</v>
       </c>
       <c r="D30" t="n">
+        <v>3.31546713</v>
+      </c>
+      <c r="E30" t="n">
         <v>3.83106848</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>4.73963403</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>2.78093982</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>7.56747288</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:8">
       <c r="A31" s="2" t="n">
         <v>43807</v>
       </c>
@@ -1088,19 +1177,22 @@
         <v>1.37390756</v>
       </c>
       <c r="D31" t="n">
+        <v>1.73886803</v>
+      </c>
+      <c r="E31" t="n">
         <v>2.41020685</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>3.51890612</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>1.03160908</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>6.593269820000001</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8">
       <c r="A32" s="2" t="n">
         <v>43808</v>
       </c>
@@ -1111,19 +1203,22 @@
         <v>3.87352538</v>
       </c>
       <c r="D32" t="n">
+        <v>4.133844509999999</v>
+      </c>
+      <c r="E32" t="n">
         <v>4.582066940000001</v>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>5.42218682</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>3.63900251</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>11.90449547</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8">
       <c r="A33" s="2" t="n">
         <v>43809</v>
       </c>
@@ -1134,19 +1229,22 @@
         <v>4.12334218</v>
       </c>
       <c r="D33" t="n">
+        <v>4.29139671</v>
+      </c>
+      <c r="E33" t="n">
         <v>4.60825475</v>
       </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
         <v>5.22861493</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>3.97343265</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>9.96935867</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8">
       <c r="A34" s="2" t="n">
         <v>43810</v>
       </c>
@@ -1157,19 +1255,22 @@
         <v>8.161415290000001</v>
       </c>
       <c r="D34" t="n">
+        <v>8.31486445</v>
+      </c>
+      <c r="E34" t="n">
         <v>8.609938810000001</v>
       </c>
-      <c r="E34" t="n">
+      <c r="F34" t="n">
         <v>9.15393493</v>
       </c>
-      <c r="F34" t="n">
+      <c r="G34" t="n">
         <v>8.015301340000001</v>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>12.27936715</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8">
       <c r="A35" s="2" t="n">
         <v>43811</v>
       </c>
@@ -1180,19 +1281,22 @@
         <v>9.158716140000001</v>
       </c>
       <c r="D35" t="n">
+        <v>9.31707134</v>
+      </c>
+      <c r="E35" t="n">
         <v>9.65930266</v>
       </c>
-      <c r="E35" t="n">
+      <c r="F35" t="n">
         <v>10.28048401</v>
       </c>
-      <c r="F35" t="n">
+      <c r="G35" t="n">
         <v>9.01382029</v>
       </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
         <v>15.97511126</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8">
       <c r="A36" s="2" t="n">
         <v>43812</v>
       </c>
@@ -1203,19 +1307,22 @@
         <v>5.17175188</v>
       </c>
       <c r="D36" t="n">
+        <v>5.36747762</v>
+      </c>
+      <c r="E36" t="n">
         <v>5.87558917</v>
       </c>
-      <c r="E36" t="n">
+      <c r="F36" t="n">
         <v>6.85137303</v>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>4.96569309</v>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>9.22502836</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:8">
       <c r="A37" s="2" t="n">
         <v>43813</v>
       </c>
@@ -1226,19 +1333,22 @@
         <v>2.17330472</v>
       </c>
       <c r="D37" t="n">
+        <v>2.50200122</v>
+      </c>
+      <c r="E37" t="n">
         <v>3.12373647</v>
       </c>
-      <c r="E37" t="n">
+      <c r="F37" t="n">
         <v>4.1551576</v>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>1.87405515</v>
       </c>
-      <c r="G37" t="n">
+      <c r="H37" t="n">
         <v>4.98191603</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:8">
       <c r="A38" s="2" t="n">
         <v>43814</v>
       </c>
@@ -1249,19 +1359,22 @@
         <v>1.31819091</v>
       </c>
       <c r="D38" t="n">
+        <v>1.68726533</v>
+      </c>
+      <c r="E38" t="n">
         <v>2.34124732</v>
       </c>
-      <c r="E38" t="n">
+      <c r="F38" t="n">
         <v>3.50403275</v>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>0.98337929</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>5.064405</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8">
       <c r="A39" s="2" t="n">
         <v>43815</v>
       </c>
@@ -1272,19 +1385,22 @@
         <v>14.41614793</v>
       </c>
       <c r="D39" t="n">
+        <v>14.54469914</v>
+      </c>
+      <c r="E39" t="n">
         <v>14.75019715</v>
       </c>
-      <c r="E39" t="n">
+      <c r="F39" t="n">
         <v>15.13178546</v>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>14.29953803</v>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>17.98381538</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8">
       <c r="A40" s="2" t="n">
         <v>43816</v>
       </c>
@@ -1295,19 +1411,22 @@
         <v>8.152994490000001</v>
       </c>
       <c r="D40" t="n">
+        <v>8.320809799999999</v>
+      </c>
+      <c r="E40" t="n">
         <v>8.64741302</v>
       </c>
-      <c r="E40" t="n">
+      <c r="F40" t="n">
         <v>9.209294720000001</v>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>7.99264361</v>
       </c>
-      <c r="G40" t="n">
+      <c r="H40" t="n">
         <v>10.61305803</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8">
       <c r="A41" s="2" t="n">
         <v>43817</v>
       </c>
@@ -1318,19 +1437,22 @@
         <v>1.54319974</v>
       </c>
       <c r="D41" t="n">
+        <v>1.93008908</v>
+      </c>
+      <c r="E41" t="n">
         <v>2.65701808</v>
       </c>
-      <c r="E41" t="n">
+      <c r="F41" t="n">
         <v>3.85591681</v>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>1.18037895</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>1.9957405</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:8">
       <c r="A42" s="2" t="n">
         <v>43818</v>
       </c>
@@ -1341,19 +1463,22 @@
         <v>1.20565428</v>
       </c>
       <c r="D42" t="n">
+        <v>1.6500187</v>
+      </c>
+      <c r="E42" t="n">
         <v>2.40883495</v>
       </c>
-      <c r="E42" t="n">
+      <c r="F42" t="n">
         <v>3.61205469</v>
       </c>
-      <c r="F42" t="n">
+      <c r="G42" t="n">
         <v>0.77384184</v>
       </c>
-      <c r="G42" t="n">
+      <c r="H42" t="n">
         <v>0.97922451</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:8">
       <c r="A43" s="2" t="n">
         <v>43819</v>
       </c>
@@ -1364,19 +1489,22 @@
         <v>1.18091702</v>
       </c>
       <c r="D43" t="n">
+        <v>1.60928411</v>
+      </c>
+      <c r="E43" t="n">
         <v>2.34736498</v>
       </c>
-      <c r="E43" t="n">
+      <c r="F43" t="n">
         <v>3.51652309</v>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
         <v>0.77192089</v>
       </c>
-      <c r="G43" t="n">
+      <c r="H43" t="n">
         <v>1.16037187</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:8">
       <c r="A44" s="2" t="n">
         <v>43820</v>
       </c>
@@ -1387,19 +1515,22 @@
         <v>1.56270601</v>
       </c>
       <c r="D44" t="n">
+        <v>1.90620747</v>
+      </c>
+      <c r="E44" t="n">
         <v>2.50019654</v>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>3.51849027</v>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>1.2265561</v>
       </c>
-      <c r="G44" t="n">
+      <c r="H44" t="n">
         <v>2.37768078</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8">
       <c r="A45" s="2" t="n">
         <v>43821</v>
       </c>
@@ -1410,19 +1541,22 @@
         <v>1.07818221</v>
       </c>
       <c r="D45" t="n">
+        <v>1.46688745</v>
+      </c>
+      <c r="E45" t="n">
         <v>2.12614449</v>
       </c>
-      <c r="E45" t="n">
+      <c r="F45" t="n">
         <v>3.16333297</v>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>0.7102626400000001</v>
       </c>
-      <c r="G45" t="n">
+      <c r="H45" t="n">
         <v>1.32963016</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:8">
       <c r="A46" s="2" t="n">
         <v>43822</v>
       </c>
@@ -1433,19 +1567,22 @@
         <v>1.13269156</v>
       </c>
       <c r="D46" t="n">
+        <v>1.54010992</v>
+      </c>
+      <c r="E46" t="n">
         <v>2.2275016</v>
       </c>
-      <c r="E46" t="n">
+      <c r="F46" t="n">
         <v>3.30867967</v>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>0.7283939399999999</v>
       </c>
-      <c r="G46" t="n">
+      <c r="H46" t="n">
         <v>1.17598025</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:8">
       <c r="A47" s="2" t="n">
         <v>43823</v>
       </c>
@@ -1456,19 +1593,22 @@
         <v>1.13427934</v>
       </c>
       <c r="D47" t="n">
+        <v>1.54648894</v>
+      </c>
+      <c r="E47" t="n">
         <v>2.24708772</v>
       </c>
-      <c r="E47" t="n">
+      <c r="F47" t="n">
         <v>3.3452107</v>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>0.7352098100000001</v>
       </c>
-      <c r="G47" t="n">
+      <c r="H47" t="n">
         <v>1.66757324</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:8">
       <c r="A48" s="2" t="n">
         <v>43824</v>
       </c>
@@ -1479,19 +1619,22 @@
         <v>1.00340009</v>
       </c>
       <c r="D48" t="n">
+        <v>1.37455285</v>
+      </c>
+      <c r="E48" t="n">
         <v>1.99651401</v>
       </c>
-      <c r="E48" t="n">
+      <c r="F48" t="n">
         <v>2.98475619</v>
       </c>
-      <c r="F48" t="n">
+      <c r="G48" t="n">
         <v>0.6394</v>
       </c>
-      <c r="G48" t="n">
+      <c r="H48" t="n">
         <v>1.12338649</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:8">
       <c r="A49" s="2" t="n">
         <v>43825</v>
       </c>
@@ -1502,19 +1645,22 @@
         <v>1.00160075</v>
       </c>
       <c r="D49" t="n">
+        <v>1.37209688</v>
+      </c>
+      <c r="E49" t="n">
         <v>1.98790958</v>
       </c>
-      <c r="E49" t="n">
+      <c r="F49" t="n">
         <v>2.97307014</v>
       </c>
-      <c r="F49" t="n">
+      <c r="G49" t="n">
         <v>0.6374555200000001</v>
       </c>
-      <c r="G49" t="n">
+      <c r="H49" t="n">
         <v>1.19237122</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:8">
       <c r="A50" s="2" t="n">
         <v>43826</v>
       </c>
@@ -1525,19 +1671,22 @@
         <v>1.01552006</v>
       </c>
       <c r="D50" t="n">
+        <v>1.38482464</v>
+      </c>
+      <c r="E50" t="n">
         <v>2.00588381</v>
       </c>
-      <c r="E50" t="n">
+      <c r="F50" t="n">
         <v>2.97952901</v>
       </c>
-      <c r="F50" t="n">
+      <c r="G50" t="n">
         <v>0.64808678</v>
       </c>
-      <c r="G50" t="n">
+      <c r="H50" t="n">
         <v>0.23041161</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:8">
       <c r="A51" s="2" t="n">
         <v>43827</v>
       </c>
@@ -1548,19 +1697,22 @@
         <v>0.8994881300000001</v>
       </c>
       <c r="D51" t="n">
+        <v>1.23516284</v>
+      </c>
+      <c r="E51" t="n">
         <v>1.7651637</v>
       </c>
-      <c r="E51" t="n">
+      <c r="F51" t="n">
         <v>2.60243142</v>
       </c>
-      <c r="F51" t="n">
+      <c r="G51" t="n">
         <v>0.57480714</v>
       </c>
-      <c r="G51" t="n">
+      <c r="H51" t="n">
         <v>0.28500636</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:8">
       <c r="A52" s="2" t="n">
         <v>43828</v>
       </c>
@@ -1571,19 +1723,22 @@
         <v>0.9216373299999999</v>
       </c>
       <c r="D52" t="n">
+        <v>1.22279961</v>
+      </c>
+      <c r="E52" t="n">
         <v>1.74127603</v>
       </c>
-      <c r="E52" t="n">
+      <c r="F52" t="n">
         <v>2.52825669</v>
       </c>
-      <c r="F52" t="n">
+      <c r="G52" t="n">
         <v>0.60664505</v>
       </c>
-      <c r="G52" t="n">
+      <c r="H52" t="n">
         <v>0.35185619</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:8">
       <c r="A53" s="2" t="n">
         <v>43829</v>
       </c>
@@ -1594,19 +1749,22 @@
         <v>1.08626775</v>
       </c>
       <c r="D53" t="n">
+        <v>1.48245372</v>
+      </c>
+      <c r="E53" t="n">
         <v>2.13863098</v>
       </c>
-      <c r="E53" t="n">
+      <c r="F53" t="n">
         <v>3.15742593</v>
       </c>
-      <c r="F53" t="n">
+      <c r="G53" t="n">
         <v>0.72261223</v>
       </c>
-      <c r="G53" t="n">
+      <c r="H53" t="n">
         <v>1.41429008</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:8">
       <c r="A54" s="2" t="n">
         <v>43830</v>
       </c>
@@ -1617,19 +1775,22 @@
         <v>1.82719719</v>
       </c>
       <c r="D54" t="n">
+        <v>2.02228318</v>
+      </c>
+      <c r="E54" t="n">
         <v>2.44938658</v>
       </c>
-      <c r="E54" t="n">
+      <c r="F54" t="n">
         <v>3.33987949</v>
       </c>
-      <c r="F54" t="n">
+      <c r="G54" t="n">
         <v>1.65593344</v>
       </c>
-      <c r="G54" t="n">
+      <c r="H54" t="n">
         <v>2.08451996</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:8">
       <c r="A55" s="2" t="n">
         <v>43831</v>
       </c>
@@ -1640,19 +1801,22 @@
         <v>1.01423518</v>
       </c>
       <c r="D55" t="n">
+        <v>1.38516056</v>
+      </c>
+      <c r="E55" t="n">
         <v>2.01730958</v>
       </c>
-      <c r="E55" t="n">
+      <c r="F55" t="n">
         <v>2.99884667</v>
       </c>
-      <c r="F55" t="n">
+      <c r="G55" t="n">
         <v>0.6517844300000001</v>
       </c>
-      <c r="G55" t="n">
+      <c r="H55" t="n">
         <v>1.05321325</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:8">
       <c r="A56" s="2" t="n">
         <v>43832</v>
       </c>
@@ -1663,19 +1827,22 @@
         <v>1.02742908</v>
       </c>
       <c r="D56" t="n">
+        <v>1.40192087</v>
+      </c>
+      <c r="E56" t="n">
         <v>2.03071605</v>
       </c>
-      <c r="E56" t="n">
+      <c r="F56" t="n">
         <v>3.02438942</v>
       </c>
-      <c r="F56" t="n">
+      <c r="G56" t="n">
         <v>0.65523438</v>
       </c>
-      <c r="G56" t="n">
+      <c r="H56" t="n">
         <v>1.5261105</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:8">
       <c r="A57" s="2" t="n">
         <v>43833</v>
       </c>
@@ -1686,19 +1853,22 @@
         <v>1.93039276</v>
       </c>
       <c r="D57" t="n">
+        <v>2.12897313</v>
+      </c>
+      <c r="E57" t="n">
         <v>2.49947718</v>
       </c>
-      <c r="E57" t="n">
+      <c r="F57" t="n">
         <v>3.42342953</v>
       </c>
-      <c r="F57" t="n">
+      <c r="G57" t="n">
         <v>1.76039605</v>
       </c>
-      <c r="G57" t="n">
+      <c r="H57" t="n">
         <v>2.85296736</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:8">
       <c r="A58" s="2" t="n">
         <v>43834</v>
       </c>
@@ -1709,19 +1879,22 @@
         <v>1.32549764</v>
       </c>
       <c r="D58" t="n">
+        <v>1.64190024</v>
+      </c>
+      <c r="E58" t="n">
         <v>2.2012289</v>
       </c>
-      <c r="E58" t="n">
+      <c r="F58" t="n">
         <v>3.18811676</v>
       </c>
-      <c r="F58" t="n">
+      <c r="G58" t="n">
         <v>1.02623647</v>
       </c>
-      <c r="G58" t="n">
+      <c r="H58" t="n">
         <v>2.19693942</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:8">
       <c r="A59" s="2" t="n">
         <v>43835</v>
       </c>
@@ -1732,19 +1905,22 @@
         <v>1.14398443</v>
       </c>
       <c r="D59" t="n">
+        <v>1.50848797</v>
+      </c>
+      <c r="E59" t="n">
         <v>2.1412278</v>
       </c>
-      <c r="E59" t="n">
+      <c r="F59" t="n">
         <v>3.18312792</v>
       </c>
-      <c r="F59" t="n">
+      <c r="G59" t="n">
         <v>0.79295735</v>
       </c>
-      <c r="G59" t="n">
+      <c r="H59" t="n">
         <v>2.13336249</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:8">
       <c r="A60" s="2" t="n">
         <v>43836</v>
       </c>
@@ -1753,11 +1929,12 @@
       <c r="D60" t="s"/>
       <c r="E60" t="s"/>
       <c r="F60" t="s"/>
-      <c r="G60" t="n">
+      <c r="G60" t="s"/>
+      <c r="H60" t="n">
         <v>2.12529366</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:8">
       <c r="A61" s="2" t="n">
         <v>43837</v>
       </c>
@@ -1768,19 +1945,22 @@
         <v>4.93368829</v>
       </c>
       <c r="D61" t="n">
+        <v>5.015849820000001</v>
+      </c>
+      <c r="E61" t="n">
         <v>5.23780738</v>
       </c>
-      <c r="E61" t="n">
+      <c r="F61" t="n">
         <v>5.89620217</v>
       </c>
-      <c r="F61" t="n">
+      <c r="G61" t="n">
         <v>4.90099748</v>
       </c>
-      <c r="G61" t="n">
+      <c r="H61" t="n">
         <v>6.72377808</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:8">
       <c r="A62" s="2" t="n">
         <v>43838</v>
       </c>
@@ -1791,19 +1971,22 @@
         <v>6.68974118</v>
       </c>
       <c r="D62" t="n">
+        <v>6.78891445</v>
+      </c>
+      <c r="E62" t="n">
         <v>6.97466771</v>
       </c>
-      <c r="E62" t="n">
+      <c r="F62" t="n">
         <v>7.452383650000001</v>
       </c>
-      <c r="F62" t="n">
+      <c r="G62" t="n">
         <v>6.59251669</v>
       </c>
-      <c r="G62" t="n">
+      <c r="H62" t="n">
         <v>8.121970660000001</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:8">
       <c r="A63" s="2" t="n">
         <v>43839</v>
       </c>
@@ -1814,19 +1997,22 @@
         <v>5.60173612</v>
       </c>
       <c r="D63" t="n">
+        <v>5.69357812</v>
+      </c>
+      <c r="E63" t="n">
         <v>5.87939745</v>
       </c>
-      <c r="E63" t="n">
+      <c r="F63" t="n">
         <v>6.40824387</v>
       </c>
-      <c r="F63" t="n">
+      <c r="G63" t="n">
         <v>5.51783043</v>
       </c>
-      <c r="G63" t="n">
+      <c r="H63" t="n">
         <v>7.1789169</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:8">
       <c r="A64" s="2" t="n">
         <v>43840</v>
       </c>
@@ -1837,19 +2023,22 @@
         <v>6.284379410000001</v>
       </c>
       <c r="D64" t="n">
+        <v>6.37937342</v>
+      </c>
+      <c r="E64" t="n">
         <v>6.57276109</v>
       </c>
-      <c r="E64" t="n">
+      <c r="F64" t="n">
         <v>6.908164559999999</v>
       </c>
-      <c r="F64" t="n">
+      <c r="G64" t="n">
         <v>6.2045203</v>
       </c>
-      <c r="G64" t="n">
+      <c r="H64" t="n">
         <v>8.240316740000001</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:8">
       <c r="A65" s="2" t="n">
         <v>43841</v>
       </c>
@@ -1860,19 +2049,22 @@
         <v>4.77032621</v>
       </c>
       <c r="D65" t="n">
+        <v>4.80706355</v>
+      </c>
+      <c r="E65" t="n">
         <v>4.94954349</v>
       </c>
-      <c r="E65" t="n">
+      <c r="F65" t="n">
         <v>5.25606335</v>
       </c>
-      <c r="F65" t="n">
+      <c r="G65" t="n">
         <v>4.74108436</v>
       </c>
-      <c r="G65" t="n">
+      <c r="H65" t="n">
         <v>6.63611967</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:8">
       <c r="A66" s="2" t="n">
         <v>43842</v>
       </c>
@@ -1883,19 +2075,22 @@
         <v>3.01924515</v>
       </c>
       <c r="D66" t="n">
+        <v>3.17962824</v>
+      </c>
+      <c r="E66" t="n">
         <v>3.39700834</v>
       </c>
-      <c r="E66" t="n">
+      <c r="F66" t="n">
         <v>4.03727893</v>
       </c>
-      <c r="F66" t="n">
+      <c r="G66" t="n">
         <v>2.89175015</v>
       </c>
-      <c r="G66" t="n">
+      <c r="H66" t="n">
         <v>3.98261109</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:8">
       <c r="A67" s="2" t="n">
         <v>43843</v>
       </c>
@@ -1906,19 +2101,22 @@
         <v>8.20217353</v>
       </c>
       <c r="D67" t="n">
+        <v>8.30505866</v>
+      </c>
+      <c r="E67" t="n">
         <v>8.43603317</v>
       </c>
-      <c r="E67" t="n">
+      <c r="F67" t="n">
         <v>8.731831339999999</v>
       </c>
-      <c r="F67" t="n">
+      <c r="G67" t="n">
         <v>8.11970874</v>
       </c>
-      <c r="G67" t="n">
+      <c r="H67" t="n">
         <v>10.62206537</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:8">
       <c r="A68" s="2" t="n">
         <v>43844</v>
       </c>
@@ -1929,19 +2127,22 @@
         <v>5.71715547</v>
       </c>
       <c r="D68" t="n">
+        <v>5.73788951</v>
+      </c>
+      <c r="E68" t="n">
         <v>5.81375883</v>
       </c>
-      <c r="E68" t="n">
+      <c r="F68" t="n">
         <v>6.03021457</v>
       </c>
-      <c r="F68" t="n">
+      <c r="G68" t="n">
         <v>5.69712171</v>
       </c>
-      <c r="G68" t="n">
+      <c r="H68" t="n">
         <v>8.811132730000001</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:8">
       <c r="A69" s="2" t="n">
         <v>43845</v>
       </c>
@@ -1952,19 +2153,22 @@
         <v>8.05441544</v>
       </c>
       <c r="D69" t="n">
+        <v>8.06228291</v>
+      </c>
+      <c r="E69" t="n">
         <v>8.071432440000001</v>
       </c>
-      <c r="E69" t="n">
+      <c r="F69" t="n">
         <v>8.104703130000001</v>
       </c>
-      <c r="F69" t="n">
+      <c r="G69" t="n">
         <v>8.04571185</v>
       </c>
-      <c r="G69" t="n">
+      <c r="H69" t="n">
         <v>11.40968027</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:8">
       <c r="A70" s="2" t="n">
         <v>43846</v>
       </c>
@@ -1975,15 +2179,18 @@
         <v>8.222550460000001</v>
       </c>
       <c r="D70" t="n">
+        <v>8.28901924</v>
+      </c>
+      <c r="E70" t="n">
         <v>8.4020835</v>
       </c>
-      <c r="E70" t="n">
+      <c r="F70" t="n">
         <v>8.58210377</v>
       </c>
-      <c r="F70" t="n">
+      <c r="G70" t="n">
         <v>8.163977639999999</v>
       </c>
-      <c r="G70" t="n">
+      <c r="H70" t="n">
         <v>12.42609189</v>
       </c>
     </row>

</xml_diff>